<commit_message>
Clean up types and schema
</commit_message>
<xml_diff>
--- a/Appointment Table.xlsx
+++ b/Appointment Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\schedular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04E1BD8-06C1-4C1E-B5F3-C897D5A22162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B6104B-DB44-46BE-8503-67E26EEFACE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="27090" windowHeight="17490" activeTab="3" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
+    <workbookView xWindow="330" yWindow="4020" windowWidth="27990" windowHeight="16710" activeTab="3" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="119">
   <si>
     <t>Attributes</t>
   </si>
@@ -317,13 +317,7 @@
     <t>/user/calendar</t>
   </si>
   <si>
-    <t>appointmentId (gsi)</t>
-  </si>
-  <si>
     <t>email (gsi)</t>
-  </si>
-  <si>
-    <t>bookingId (gsi)</t>
   </si>
   <si>
     <t>status = (booked or cancelled)</t>
@@ -464,9 +458,6 @@
     <t>cancelled</t>
   </si>
   <si>
-    <t>{ pk, sk, duration, type, category }</t>
-  </si>
-  <si>
     <t>smith#john</t>
   </si>
   <si>
@@ -493,6 +484,12 @@
   </si>
   <si>
     <t>type = appt, SK between &lt;date1&gt; and &lt;date2&gt;</t>
+  </si>
+  <si>
+    <t>bookingId</t>
+  </si>
+  <si>
+    <t>{ pk, sk, status, type, category, duration }</t>
   </si>
 </sst>
 </file>
@@ -534,7 +531,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,6 +547,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,7 +586,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -676,11 +679,17 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1249,10 +1258,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
@@ -1273,10 +1282,10 @@
         <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="6" t="s">
@@ -1291,16 +1300,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6" t="s">
@@ -1315,16 +1324,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="6" t="s">
@@ -1345,7 +1354,7 @@
         <v>47</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="6" t="s">
@@ -1366,10 +1375,10 @@
         <v>47</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>20</v>
@@ -1389,10 +1398,10 @@
         <v>47</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>64</v>
@@ -1412,7 +1421,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,9 +1430,10 @@
     <col min="2" max="2" width="33.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.28515625" style="22" bestFit="1" customWidth="1"/>
@@ -1431,18 +1441,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -1457,12 +1467,12 @@
       <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1470,11 +1480,11 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>89</v>
+      <c r="B3" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>11</v>
@@ -1483,13 +1493,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>67</v>
+      <c r="G3" s="34" t="s">
+        <v>117</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>54</v>
@@ -1499,8 +1509,8 @@
       <c r="N3" s="19"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1513,21 +1523,21 @@
       <c r="F4" s="7">
         <v>60</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="35" t="s">
         <v>57</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L4" s="21"/>
       <c r="N4" s="22"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>89</v>
+      <c r="B5" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>11</v>
@@ -1536,15 +1546,12 @@
         <v>14</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="16" t="s">
         <v>54</v>
       </c>
       <c r="J5" s="21"/>
@@ -1554,25 +1561,22 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="20"/>
@@ -1581,11 +1585,11 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>90</v>
+      <c r="B7" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>11</v>
@@ -1594,7 +1598,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>10</v>
@@ -1605,8 +1609,8 @@
       <c r="N7" s="22"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1625,11 +1629,11 @@
       <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>90</v>
+      <c r="B9" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>11</v>
@@ -1638,15 +1642,12 @@
         <v>14</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>56</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="16" t="s">
         <v>54</v>
       </c>
       <c r="J9" s="21"/>
@@ -1657,25 +1658,22 @@
       <c r="P9" s="24"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="20"/>
@@ -1685,11 +1683,11 @@
       <c r="P10" s="24"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>90</v>
+      <c r="B11" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>11</v>
@@ -1698,15 +1696,12 @@
         <v>14</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>56</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="16" t="s">
         <v>54</v>
       </c>
       <c r="J11" s="21"/>
@@ -1717,25 +1712,22 @@
       <c r="P11" s="24"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="20"/>
@@ -1745,11 +1737,11 @@
       <c r="P12" s="24"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>91</v>
+      <c r="B13" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>11</v>
@@ -1758,7 +1750,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>10</v>
@@ -1770,8 +1762,8 @@
       <c r="O13" s="23"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1791,11 +1783,11 @@
       <c r="O14" s="22"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="33" t="s">
-        <v>92</v>
+      <c r="B15" s="32" t="s">
+        <v>90</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>11</v>
@@ -1804,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>10</v>
@@ -1816,8 +1808,8 @@
       <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="5" t="s">
         <v>22</v>
       </c>
@@ -1837,11 +1829,11 @@
       <c r="O16" s="22"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="33" t="s">
-        <v>93</v>
+      <c r="B17" s="32" t="s">
+        <v>91</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>11</v>
@@ -1850,7 +1842,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>10</v>
@@ -1862,8 +1854,8 @@
       <c r="O17" s="22"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
@@ -1883,11 +1875,11 @@
       <c r="O18" s="22"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>111</v>
+      <c r="B19" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>59</v>
@@ -1896,7 +1888,7 @@
         <v>60</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>61</v>
@@ -1908,16 +1900,16 @@
       <c r="O19" s="22"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F20" s="7">
         <v>7805555555</v>
@@ -1927,11 +1919,11 @@
       <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>115</v>
+      <c r="B21" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>59</v>
@@ -1940,7 +1932,7 @@
         <v>60</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>61</v>
@@ -1952,16 +1944,16 @@
       <c r="O21" s="22"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F22" s="7">
         <v>7808888888</v>
@@ -1996,7 +1988,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I25" s="27" t="s">
         <v>51</v>
@@ -2010,7 +2002,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>50</v>
@@ -2022,7 +2014,7 @@
         <v>47</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28" t="s">
@@ -2035,7 +2027,7 @@
     </row>
     <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>24</v>
@@ -2047,16 +2039,16 @@
         <v>46</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>25</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I27" s="28" t="s">
         <v>13</v>
@@ -2068,7 +2060,7 @@
     </row>
     <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>48</v>
@@ -2080,13 +2072,13 @@
         <v>46</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I28" s="28" t="s">
         <v>52</v>
@@ -2098,10 +2090,10 @@
     </row>
     <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>49</v>
@@ -2110,7 +2102,7 @@
         <v>47</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
@@ -2120,33 +2112,33 @@
         <v>19</v>
       </c>
       <c r="K29" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E30" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="28" t="s">
         <v>105</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>107</v>
       </c>
       <c r="I30" s="28" t="s">
         <v>26</v>
@@ -2158,10 +2150,10 @@
     </row>
     <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>49</v>
@@ -2170,7 +2162,7 @@
         <v>47</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28" t="s">
@@ -2180,7 +2172,7 @@
         <v>19</v>
       </c>
       <c r="K31" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2192,6 +2184,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="A21:A22"/>
@@ -2202,18 +2206,6 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1" xr:uid="{B610ACA8-BB27-4EB4-9FA5-FD775FD9DEC9}"/>

</xml_diff>